<commit_message>
DRC - pass, testpoints, draftsman pdf, gerbers.
</commit_message>
<xml_diff>
--- a/Electronics/AltiumProject/Rad_hard_git/Project Outputs for Rad_hard_git/Rad_hard_git.xlsx
+++ b/Electronics/AltiumProject/Rad_hard_git/Project Outputs for Rad_hard_git/Rad_hard_git.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="197">
   <si>
     <t>Comment</t>
   </si>
@@ -39,147 +39,195 @@
     <t>Quantity</t>
   </si>
   <si>
+    <t>Component_1</t>
+  </si>
+  <si>
+    <t>Amph</t>
+  </si>
+  <si>
+    <t>PCBComponent_1</t>
+  </si>
+  <si>
     <t>ACRK-16-01-G-T-B1-M-1</t>
   </si>
   <si>
-    <t>PCBComponent_1</t>
-  </si>
-  <si>
-    <t>Component_1</t>
+    <t>MAL214099801E3</t>
+  </si>
+  <si>
+    <t>No Description Available</t>
+  </si>
+  <si>
+    <t>C1, C2, C3, C10, C11, C12, C13</t>
+  </si>
+  <si>
+    <t>CAP_140CRH_1010_VIS</t>
+  </si>
+  <si>
+    <t>12065A5R6DAT2A</t>
+  </si>
+  <si>
+    <t>CAP CER 5.6PF 50V C0G/NP0 1206</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>CAPC3216X94N</t>
+  </si>
+  <si>
+    <t>CC0603KRX7R7BB105</t>
+  </si>
+  <si>
+    <t>CAP CER 1UF 16V X7R 0603</t>
+  </si>
+  <si>
+    <t>C5, C6, C14, C15, C16</t>
+  </si>
+  <si>
+    <t>FP-CC0603-DA-MFG</t>
+  </si>
+  <si>
+    <t>CMP-03422-000924-1</t>
+  </si>
+  <si>
+    <t>06033C104KAT2A</t>
+  </si>
+  <si>
+    <t>General Purpose Ceramic Capacitor, 0603, 100nF, 10%, X7R, 15%, 25V</t>
+  </si>
+  <si>
+    <t>C7, C8</t>
+  </si>
+  <si>
+    <t>FP-0603-L_1_6_0_15-W_0_81-MFG</t>
+  </si>
+  <si>
+    <t>CMP-2006-04157-2</t>
+  </si>
+  <si>
+    <t>VJ0805Y223KXXAC</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>CAPC2012X145N</t>
+  </si>
+  <si>
+    <t>GRM31CR71E106KA12L</t>
+  </si>
+  <si>
+    <t>Chip Multilayer Ceramic Capacitors for General Purpose, 1206, 10uF, X7R, 15%, 10%, 25V</t>
+  </si>
+  <si>
+    <t>C17, C18, C19, C20</t>
+  </si>
+  <si>
+    <t>FP-GRM31C-0_2-e0_3_0_8-MFG</t>
+  </si>
+  <si>
+    <t>CMP-06035-003589-1</t>
+  </si>
+  <si>
+    <t>CC0402KRX7R9BB104</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 50V X7R 0402</t>
+  </si>
+  <si>
+    <t>C21_Temperature_Enhanced_WB1, C21_Temperature_Enhanced_WB2, C22_Temperature_Enhanced_WB1, C22_Temperature_Enhanced_WB2, C23_Temperature_Enhanced_WB1, C23_Temperature_Enhanced_WB2</t>
+  </si>
+  <si>
+    <t>FP-CC0402-MFG</t>
+  </si>
+  <si>
+    <t>CMP-03422-001010-1</t>
+  </si>
+  <si>
+    <t>PTVS12VP1UP,115</t>
+  </si>
+  <si>
+    <t>Diode ESD (Uni-directional)</t>
+  </si>
+  <si>
+    <t>D1, D2, D5, D6, D11, D12, D17, D18</t>
+  </si>
+  <si>
+    <t>PMEG3050EP115</t>
+  </si>
+  <si>
+    <t>YQ15RSM10SDTL1</t>
+  </si>
+  <si>
+    <t>Schottky Diode</t>
+  </si>
+  <si>
+    <t>D3, D4, D7, D15, D16, D19, D20</t>
+  </si>
+  <si>
+    <t>VBPW34S</t>
+  </si>
+  <si>
+    <t>VBPW34SR Series 60 V 940 nm 50 mA 215 mW Surface Mount Silicon PIN Photodiode</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>XDCR_VBPW34S</t>
+  </si>
+  <si>
+    <t>RF05VYM1SFHTR</t>
+  </si>
+  <si>
+    <t>Diode</t>
+  </si>
+  <si>
+    <t>D9, D10, D21, D22, D23_Temperature_Enhanced_WB1, D23_Temperature_Enhanced_WB2, D24_Temperature_Enhanced_WB1, D24_Temperature_Enhanced_WB2, D25_Temperature_Enhanced_WB1, D25_Temperature_Enhanced_WB2, D26_Temperature_Enhanced_WB1, D26_Temperature_Enhanced_WB2</t>
+  </si>
+  <si>
+    <t>0483005.DR</t>
+  </si>
+  <si>
+    <t>Fuse</t>
+  </si>
+  <si>
+    <t>F1, F3</t>
+  </si>
+  <si>
+    <t>FUSC3316X137N</t>
+  </si>
+  <si>
+    <t>0483010.DR</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>MH1608-601Y</t>
+  </si>
+  <si>
+    <t>FERRITE BEAD 600 OHM 0603 1LN</t>
+  </si>
+  <si>
+    <t>FB1, FB2</t>
+  </si>
+  <si>
+    <t>FP-MH1608-MFG</t>
+  </si>
+  <si>
+    <t>CMP-2000-06698-2</t>
+  </si>
+  <si>
+    <t>GUARD_RING</t>
+  </si>
+  <si>
+    <t>GR</t>
   </si>
   <si>
     <t>Guard</t>
   </si>
   <si>
-    <t>Capacitor</t>
-  </si>
-  <si>
-    <t>C1, C2, C3</t>
-  </si>
-  <si>
-    <t>12065A5R6DAT2A</t>
-  </si>
-  <si>
-    <t>CAP CER 5.6PF 50V C0G/NP0 1206</t>
-  </si>
-  <si>
-    <t>C4</t>
-  </si>
-  <si>
-    <t>CAPC3216X94N</t>
-  </si>
-  <si>
-    <t>CC0603KRX7R7BB105</t>
-  </si>
-  <si>
-    <t>CAP CER 1UF 16V X7R 0603</t>
-  </si>
-  <si>
-    <t>C5, C6</t>
-  </si>
-  <si>
-    <t>FP-CC0603-DA-MFG</t>
-  </si>
-  <si>
-    <t>CMP-03422-000924-1</t>
-  </si>
-  <si>
-    <t>06033C104KAT2A</t>
-  </si>
-  <si>
-    <t>General Purpose Ceramic Capacitor, 0603, 100nF, 10%, X7R, 15%, 25V</t>
-  </si>
-  <si>
-    <t>C7, C8</t>
-  </si>
-  <si>
-    <t>FP-0603-L_1_6_0_15-W_0_81-MFG</t>
-  </si>
-  <si>
-    <t>CMP-2006-04157-2</t>
-  </si>
-  <si>
-    <t>PTVS12VP1UP,115</t>
-  </si>
-  <si>
-    <t>Diode ESD (Uni-directional)</t>
-  </si>
-  <si>
-    <t>D1, D2, D5, D6, D11, D12, D13, D14</t>
-  </si>
-  <si>
-    <t>PMEG3050EP115</t>
-  </si>
-  <si>
-    <t>YQ15RSM10SDTL1</t>
-  </si>
-  <si>
-    <t>Schottky Diode</t>
-  </si>
-  <si>
-    <t>D3, D4, D7</t>
-  </si>
-  <si>
-    <t>BPW_34_SR-Z</t>
-  </si>
-  <si>
-    <t>Silicon PIN Photodiode</t>
-  </si>
-  <si>
-    <t>D8</t>
-  </si>
-  <si>
-    <t>DIO_BPW_34_SR-Z</t>
-  </si>
-  <si>
-    <t>1N4148WS-E3-08</t>
-  </si>
-  <si>
-    <t>Small Signal Fast Switching Diode, 1.2 V, 350 mA, -55 to 150 degC, 2-Pin SOD-323, RoHS, Tape and Reel</t>
-  </si>
-  <si>
-    <t>D9, D10</t>
-  </si>
-  <si>
-    <t>VISH-SOD-323-2_V</t>
-  </si>
-  <si>
-    <t>CMP-2000-05517-2</t>
-  </si>
-  <si>
-    <t>0483005.DR</t>
-  </si>
-  <si>
-    <t>Fuse</t>
-  </si>
-  <si>
-    <t>F1, F3</t>
-  </si>
-  <si>
-    <t>FUSC3316X137N</t>
-  </si>
-  <si>
-    <t>0483010.DR</t>
-  </si>
-  <si>
-    <t>F2</t>
-  </si>
-  <si>
-    <t>MH1608-601Y</t>
-  </si>
-  <si>
-    <t>FERRITE BEAD 600 OHM 0603 1LN</t>
-  </si>
-  <si>
-    <t>FB1, FB2</t>
-  </si>
-  <si>
-    <t>FP-MH1608-MFG</t>
-  </si>
-  <si>
-    <t>CMP-2000-06698-2</t>
-  </si>
-  <si>
     <t>MDBRA26PEAN0</t>
   </si>
   <si>
@@ -213,12 +261,30 @@
     <t>Inductor</t>
   </si>
   <si>
-    <t>L1</t>
+    <t>L1, L2, L3</t>
   </si>
   <si>
     <t>SER8052402MEC</t>
   </si>
   <si>
+    <t>SMLD12EN1WT86C</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>LED1</t>
+  </si>
+  <si>
+    <t>SML-P11DTT86R</t>
+  </si>
+  <si>
+    <t>LED2</t>
+  </si>
+  <si>
+    <t>SML-P11(1X0.6)</t>
+  </si>
+  <si>
     <t>UJ4SC075018B7S</t>
   </si>
   <si>
@@ -228,19 +294,16 @@
     <t>Q1, Q6</t>
   </si>
   <si>
-    <t>2N2222A</t>
-  </si>
-  <si>
-    <t>High Speed Switch, 0.6 A IC, -65 to 175 degC, 3-Pin TO-18, RoHS, Bulk</t>
-  </si>
-  <si>
-    <t>Q2, Q3, Q4, Q8, Q9, Q10, Q11, Q12, Q13</t>
-  </si>
-  <si>
-    <t>STM-TO-18-3</t>
-  </si>
-  <si>
-    <t>CMP-2000-05381-1</t>
+    <t>2SD1834T100</t>
+  </si>
+  <si>
+    <t>Transistor BJT NPN</t>
+  </si>
+  <si>
+    <t>Q2, Q3, Q4, Q8, Q9, Q10, Q11, Q12, Q14, Q15</t>
+  </si>
+  <si>
+    <t>RJP020N06</t>
   </si>
   <si>
     <t>IXTA6N100D2</t>
@@ -255,6 +318,15 @@
     <t>DPAK254P1524X483-3N</t>
   </si>
   <si>
+    <t>2SCR563F3TR</t>
+  </si>
+  <si>
+    <t>Q13</t>
+  </si>
+  <si>
+    <t>2SAR542F3</t>
+  </si>
+  <si>
     <t>LT5400ACMS8E-3#PBF</t>
   </si>
   <si>
@@ -273,91 +345,175 @@
     <t>R2</t>
   </si>
   <si>
+    <t>WSLP0805R0100FEA</t>
+  </si>
+  <si>
+    <t>R3, R9</t>
+  </si>
+  <si>
+    <t>RESC2013X58X38LL25T25</t>
+  </si>
+  <si>
+    <t>CMP-2001-04321-1</t>
+  </si>
+  <si>
+    <t>ERA8AEB124V</t>
+  </si>
+  <si>
+    <t>R4, R7, R10, R11</t>
+  </si>
+  <si>
+    <t>RESC3216X70X50LL20T25</t>
+  </si>
+  <si>
+    <t>CMP-2003-04417-1</t>
+  </si>
+  <si>
+    <t>MCT06030C1001FP500</t>
+  </si>
+  <si>
+    <t>Res Thin Film 0603 1K Ohm 1% 0.1W(1/10W) ?50ppm/C Molded SMD Automotive Medical T/R</t>
+  </si>
+  <si>
+    <t>R5, R6, R8, R12, R13, R14, R15, R17, R19, R21, R30, R34, R35, R50_Temperature_Enhanced_WB1, R50_Temperature_Enhanced_WB2, R53_Temperature_Enhanced_WB1, R53_Temperature_Enhanced_WB2, R54_Temperature_Enhanced_WB1, R54_Temperature_Enhanced_WB2, R55, R56</t>
+  </si>
+  <si>
+    <t>RESC1508X55N</t>
+  </si>
+  <si>
+    <t>ERJ-8GEYJ241V</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>RESC3216X70X50NL05T20</t>
+  </si>
+  <si>
+    <t>CMP-2003-00592-1</t>
+  </si>
+  <si>
+    <t>CRHP1206AF1G00FKET</t>
+  </si>
+  <si>
+    <t>R18</t>
+  </si>
+  <si>
+    <t>RES_CRHP1206_VIS</t>
+  </si>
+  <si>
+    <t>MCT06030C1004FPW00</t>
+  </si>
+  <si>
+    <t>RES SMD 100 OHM 1% 1/8W 0603</t>
+  </si>
+  <si>
+    <t>R22, R23, R24, R26</t>
+  </si>
+  <si>
+    <t>FP-MCT0603-MFG</t>
+  </si>
+  <si>
+    <t>CMP-02407-007592-1</t>
+  </si>
+  <si>
+    <t>UPF50B100RV</t>
+  </si>
+  <si>
+    <t>R25</t>
+  </si>
+  <si>
+    <t>RES_UPF50B2K0V_TEC</t>
+  </si>
+  <si>
+    <t>0402WGF1000TCE</t>
+  </si>
+  <si>
     <t>Resistor</t>
   </si>
   <si>
-    <t>R3, R9</t>
-  </si>
-  <si>
-    <t>ERA8AEB124V</t>
-  </si>
-  <si>
-    <t>R4, R7, R10, R11</t>
-  </si>
-  <si>
-    <t>RESC3216X70X50LL20T25</t>
-  </si>
-  <si>
-    <t>CMP-2003-04417-1</t>
-  </si>
-  <si>
-    <t>MCT06030C1001FP500</t>
-  </si>
-  <si>
-    <t>Res Thin Film 0603 1K Ohm 1% 0.1W(1/10W) ?50ppm/C Molded SMD Automotive Medical T/R</t>
-  </si>
-  <si>
-    <t>R5, R6, R8, R12, R13, R14, R15, R17, R19, R21</t>
-  </si>
-  <si>
-    <t>RESC1508X55N</t>
-  </si>
-  <si>
-    <t>ERJ-8GEYJ241V</t>
-  </si>
-  <si>
-    <t>R16</t>
-  </si>
-  <si>
-    <t>RESC3216X70X50NL05T20</t>
-  </si>
-  <si>
-    <t>CMP-2003-00592-1</t>
-  </si>
-  <si>
-    <t>CRHP1206AF1G00FKET</t>
-  </si>
-  <si>
-    <t>No Description Available</t>
-  </si>
-  <si>
-    <t>R18</t>
-  </si>
-  <si>
-    <t>RES_CRHP1206_VIS</t>
-  </si>
-  <si>
-    <t>MCT06030C1004FPW00</t>
-  </si>
-  <si>
-    <t>RES SMD 100 OHM 1% 1/8W 0603</t>
-  </si>
-  <si>
-    <t>R22, R23, R24, R26</t>
-  </si>
-  <si>
-    <t>FP-MCT0603-MFG</t>
-  </si>
-  <si>
-    <t>CMP-02407-007592-1</t>
-  </si>
-  <si>
-    <t>UPF50B100RV</t>
-  </si>
-  <si>
-    <t>R25</t>
-  </si>
-  <si>
-    <t>RES_UPF50B2K0V_TEC</t>
-  </si>
-  <si>
-    <t>MCT06030C2400FP500</t>
-  </si>
-  <si>
-    <t>R?</t>
-  </si>
-  <si>
-    <t>CMP-02407-000943-1</t>
+    <t>R27</t>
+  </si>
+  <si>
+    <t>RESC1005X40N</t>
+  </si>
+  <si>
+    <t>TNPW0603120KBEEA</t>
+  </si>
+  <si>
+    <t>R28, R29</t>
+  </si>
+  <si>
+    <t>TNPW060310K0BEEA</t>
+  </si>
+  <si>
+    <t>R31</t>
+  </si>
+  <si>
+    <t>RESC1609X55X30NL10T20</t>
+  </si>
+  <si>
+    <t>CMP-2000-03691-1</t>
+  </si>
+  <si>
+    <t>PTS1206M2B1K00P100</t>
+  </si>
+  <si>
+    <t>R32</t>
+  </si>
+  <si>
+    <t>PTS 1206_VIS</t>
+  </si>
+  <si>
+    <t>3214W-1-502E</t>
+  </si>
+  <si>
+    <t>3214 - 5-Turn Trimpot(R) Trimming Potentiometer, 5 KOhm, +/- 10%, 0.25 W, -65 to 150 degC, RoHS, Tape and Reel</t>
+  </si>
+  <si>
+    <t>R33</t>
+  </si>
+  <si>
+    <t>BOUR-3214W_V</t>
+  </si>
+  <si>
+    <t>CMP-2000-05579-1</t>
+  </si>
+  <si>
+    <t>H810KBYA</t>
+  </si>
+  <si>
+    <t>R36_Temperature_Enhanced_WB1, R36_Temperature_Enhanced_WB2, R37_Temperature_Enhanced_WB1, R37_Temperature_Enhanced_WB2</t>
+  </si>
+  <si>
+    <t>RESAD1690W60L710D245</t>
+  </si>
+  <si>
+    <t>H81M0BYA</t>
+  </si>
+  <si>
+    <t>R38_Temperature_Enhanced_WB1, R38_Temperature_Enhanced_WB2, R39_Temperature_Enhanced_WB1, R39_Temperature_Enhanced_WB2</t>
+  </si>
+  <si>
+    <t>H81K0BYA</t>
+  </si>
+  <si>
+    <t>R40_Temperature_Enhanced_WB1, R40_Temperature_Enhanced_WB2, R45_Temperature_Enhanced_WB1, R45_Temperature_Enhanced_WB2, R46_Temperature_Enhanced_WB1, R46_Temperature_Enhanced_WB2, R49_Temperature_Enhanced_WB1, R49_Temperature_Enhanced_WB2, R51_Temperature_Enhanced_WB1, R51_Temperature_Enhanced_WB2, R52_Temperature_Enhanced_WB1, R52_Temperature_Enhanced_WB2</t>
+  </si>
+  <si>
+    <t>UPF50B100KV</t>
+  </si>
+  <si>
+    <t>R41_Temperature_Enhanced_WB1, R41_Temperature_Enhanced_WB2, R42_Temperature_Enhanced_WB1, R42_Temperature_Enhanced_WB2, R43_Temperature_Enhanced_WB1, R43_Temperature_Enhanced_WB2, R44_Temperature_Enhanced_WB1, R44_Temperature_Enhanced_WB2, R47_Temperature_Enhanced_WB1, R47_Temperature_Enhanced_WB2, R48_Temperature_Enhanced_WB1, R48_Temperature_Enhanced_WB2</t>
+  </si>
+  <si>
+    <t>5019</t>
+  </si>
+  <si>
+    <t>TP1, TP2, TP3, TP9, TP10, TP11, TP13, TP16, TP17</t>
+  </si>
+  <si>
+    <t>KEYSTONE_5019</t>
   </si>
   <si>
     <t>CH4659-ALD</t>
@@ -369,6 +525,21 @@
     <t>CH4659-ALD_COC</t>
   </si>
   <si>
+    <t>LT3045EMSE#TRPBF</t>
+  </si>
+  <si>
+    <t>IC REG LINEAR 0V 500MA 12MSOP</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>FP-MSE-12-05-08-1666-IPC_B</t>
+  </si>
+  <si>
+    <t>CMP-09138-000053-1</t>
+  </si>
+  <si>
     <t>LTZ1000ACH#PBF</t>
   </si>
   <si>
@@ -390,7 +561,7 @@
     <t>IC OPAMP ZERO-DRIFT 4CIRC 14SOIC</t>
   </si>
   <si>
-    <t>U4</t>
+    <t>U4, U6_Temperature_Enhanced_WB1, U6_Temperature_Enhanced_WB2, U9</t>
   </si>
   <si>
     <t>FP-R-14-IPC_C</t>
@@ -408,31 +579,34 @@
     <t>SOIC127P600X175-8N</t>
   </si>
   <si>
-    <t>AD713JRZ-16</t>
-  </si>
-  <si>
-    <t>Quad Channel Operational Amplifier, 4 MHz BW, 20 V/us SR, Commercial, 16-pin SOIC (RW-16), Tube</t>
-  </si>
-  <si>
-    <t>U?</t>
-  </si>
-  <si>
-    <t>ADI-RW-16_L</t>
-  </si>
-  <si>
-    <t>CMP-0384-02022-1</t>
-  </si>
-  <si>
-    <t>LM35CZ/NOPB</t>
-  </si>
-  <si>
-    <t>Precision Centigrade Temperature Sensor, 3-pin TO-92, Pb-Free</t>
-  </si>
-  <si>
-    <t>LP0003A</t>
-  </si>
-  <si>
-    <t>CMP-0066-00032-3</t>
+    <t>LT3094EMSE#PBF</t>
+  </si>
+  <si>
+    <t>IC REG LIN NEG ADJ 500MA 12MSOP</t>
+  </si>
+  <si>
+    <t>U7</t>
+  </si>
+  <si>
+    <t>FP-MSE-12-05-08-1666-MFG</t>
+  </si>
+  <si>
+    <t>CMP-09138-000010-1</t>
+  </si>
+  <si>
+    <t>ADG452BRZ</t>
+  </si>
+  <si>
+    <t>IC SWITCH QUAD SPST 16SOIC</t>
+  </si>
+  <si>
+    <t>U8_Temperature_Enhanced_WB1, U8_Temperature_Enhanced_WB2</t>
+  </si>
+  <si>
+    <t>FP-R-16-IPC_B</t>
+  </si>
+  <si>
+    <t>CMP-09113-000001-1</t>
   </si>
 </sst>
 </file>
@@ -709,7 +883,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr/>
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView view="normal" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" sqref="A1"/>
@@ -717,7 +891,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" baseColWidth="0"/>
   <cols>
-    <col min="1" max="6" width="20.0546875" customWidth="1"/>
+    <col min="1" max="6" width="20.2109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -744,15 +918,15 @@
       <c r="A2" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="19" t="s">
+        <v>8</v>
+      </c>
       <c r="D2" s="19" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="21">
         <v>1</v>
@@ -760,77 +934,79 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="27" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="17"/>
+        <v>12</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>13</v>
+      </c>
       <c r="D3" s="16" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E3" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="17">
         <v>7</v>
-      </c>
-      <c r="F3" s="17">
-        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="27" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F4" s="17">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="27" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="F5" s="17">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="27" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="F6" s="17">
         <v>2</v>
@@ -838,159 +1014,157 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>23</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B7" s="17"/>
       <c r="C7" s="16" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F7" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="27" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="F8" s="17">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="27" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="F9" s="17">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="27" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="F10" s="17">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="27" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F11" s="17">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="27" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="F12" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="27" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="F13" s="17">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="27" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F14" s="17">
         <v>2</v>
@@ -998,19 +1172,19 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="27" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F15" s="17">
         <v>1</v>
@@ -1018,39 +1192,37 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="27" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="F16" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>1</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="B17" s="17"/>
       <c r="C17" s="16" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>60</v>
+        <v>7</v>
       </c>
       <c r="F17" s="17">
         <v>1</v>
@@ -1058,19 +1230,19 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="27" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="F18" s="17">
         <v>1</v>
@@ -1078,99 +1250,95 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>68</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="B19" s="17"/>
       <c r="C19" s="16" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="F19" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>71</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="B20" s="17"/>
       <c r="C20" s="16" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F20" s="17">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="27" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F21" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="27" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="F22" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="27" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F23" s="17">
         <v>1</v>
@@ -1178,19 +1346,19 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="27" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>1</v>
+        <v>89</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="F24" s="17">
         <v>2</v>
@@ -1198,59 +1366,59 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="27" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>1</v>
+        <v>93</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F25" s="17">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="27" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="F26" s="17">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="27" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>1</v>
+        <v>93</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F27" s="17">
         <v>1</v>
@@ -1258,33 +1426,33 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="27" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="F28" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="27" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B29" s="16" t="s">
         <v>104</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D29" s="16" t="s">
         <v>106</v>
@@ -1293,84 +1461,82 @@
         <v>107</v>
       </c>
       <c r="F29" s="17">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="27" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="F30" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="27" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>104</v>
+        <v>1</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="F31" s="17">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="27" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="F32" s="17">
-        <v>1</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="27" t="s">
-        <v>117</v>
-      </c>
-      <c r="B33" s="16" t="s">
-        <v>118</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="B33" s="17"/>
       <c r="C33" s="16" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="F33" s="17">
         <v>1</v>
@@ -1378,19 +1544,19 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="27" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>123</v>
+        <v>12</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D34" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="E34" s="16" t="s">
         <v>125</v>
-      </c>
-      <c r="E34" s="16" t="s">
-        <v>126</v>
       </c>
       <c r="F34" s="17">
         <v>1</v>
@@ -1398,62 +1564,378 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="27" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>1</v>
+        <v>129</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="F35" s="17">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="27" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>131</v>
+        <v>12</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D36" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="E36" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="E36" s="16" t="s">
-        <v>134</v>
-      </c>
       <c r="F36" s="17">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="E37" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="F37" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="E38" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="F38" s="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="B39" s="17"/>
+      <c r="C39" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="E39" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="F39" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="E40" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="F40" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="E41" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="F41" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="F42" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="D43" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="E43" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="F43" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="C44" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="D44" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="E44" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="F44" s="17">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="D45" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="B37" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="C37" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="D37" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="E37" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="F37" s="17">
-        <v>1</v>
+      <c r="E45" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="F45" s="17">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="D46" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="E46" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="F46" s="17">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="D47" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="E47" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="F47" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="C48" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="D48" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="E48" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="F48" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="B49" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="C49" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="D49" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="E49" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="F49" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="C50" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="D50" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="E50" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="F50" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B51" s="17"/>
+      <c r="C51" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="D51" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="E51" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="F51" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="27" t="s">
+        <v>187</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="C52" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="D52" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="E52" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="F52" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="C53" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="D53" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="E53" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="F53" s="17">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>